<commit_message>
8/16 Points SSX Tricky Patch Research
</commit_message>
<xml_diff>
--- a/Research_Dump/Bézier Surface Patches/TrickyPS2.xlsx
+++ b/Research_Dump/Bézier Surface Patches/TrickyPS2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="7800" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patch 36" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="20">
   <si>
     <t>Playstation</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Playstation WM</t>
   </si>
   <si>
-    <t>What I need</t>
-  </si>
-  <si>
-    <t>EQ1</t>
-  </si>
-  <si>
     <t>Works</t>
   </si>
   <si>
@@ -84,12 +78,21 @@
   <si>
     <t>https://web.archive.org/web/20021105121623id_/http://www.gamasutra.com:80/gdc2002/features/rayner/rayner_pfv.htm</t>
   </si>
+  <si>
+    <t>What I need from top point</t>
+  </si>
+  <si>
+    <t>From Control</t>
+  </si>
+  <si>
+    <t>From Left Point</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +114,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +139,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -190,13 +205,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -208,9 +239,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -232,9 +265,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5200650" cy="1125693"/>
     <xdr:sp macro="" textlink="">
@@ -244,7 +277,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="47625" y="7210424"/>
+          <a:off x="57150" y="6219824"/>
           <a:ext cx="5200650" cy="1125693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -456,29 +489,35 @@
           </a:br>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
-            <a:t>Eq1 C + P1/3 = PP1</a:t>
+            <a:t>Eq1 C + P2/3 = PP2</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
           </a:br>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
-            <a:t>Eq2 PP1 + (P1+P2)/3 = PP2</a:t>
+            <a:t>Eq2 PP2 + (P2+P3)/3 = PP3</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
           </a:br>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
-            <a:t>Eq3 C + P1 +P2 +P3 = PP3</a:t>
+            <a:t>Eq3 C + P2 +P3 +P4 = PP4</a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-AU" sz="1100" baseline="0"/>
           </a:br>
-          <a:endParaRPr lang="en-AU" sz="1100" baseline="0"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t>Eq4 C + (P5 + P2 + P6/3)/3 = PP6 </a:t>
+          </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-AU" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100"/>
+            <a:t>s</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -753,7 +792,7 @@
   <dimension ref="A1:AQ32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,12 +1577,18 @@
         <f t="shared" si="4"/>
         <v>-3514.4923333333331</v>
       </c>
-      <c r="E12" s="8">
-        <f>E11+E4/3</f>
+      <c r="E12" s="1">
+        <f>B11+(B4+E3+E4/3)/3</f>
         <v>-694.7553333333334</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="1">
+        <f t="shared" ref="F12:G12" si="5">C11+(C4+F3+F4/3)/3</f>
+        <v>-96.835600111111106</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="5"/>
+        <v>-3514.4923344444442</v>
+      </c>
       <c r="H12" s="8">
         <f>H11+H4/3</f>
         <v>166.87423333333322</v>
@@ -1566,27 +1611,27 @@
         <v>-1502.1690000000001</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:D13" si="5">C12+(C4+C5)/3</f>
+        <f t="shared" ref="C13:D13" si="6">C12+(C4+C5)/3</f>
         <v>-96.835599999999999</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-4490.8125666666665</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" ref="E13:E14" si="6">E12+E5/3</f>
+        <f t="shared" ref="E13:E14" si="7">E12+E5/3</f>
         <v>-694.7553333333334</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
       <c r="H13" s="8">
-        <f t="shared" ref="H13:H14" si="7">H12+H5/3</f>
+        <f t="shared" ref="H13:H14" si="8">H12+H5/3</f>
         <v>166.87423333333322</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="8">
-        <f>K11+K5/3</f>
+        <f>K12+K5/3</f>
         <v>382.16179999999991</v>
       </c>
       <c r="L13" s="5"/>
@@ -1601,21 +1646,21 @@
         <v>-1502.1690000000001</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ref="C14:D14" si="8">C3+C4+C5+C6</f>
+        <f t="shared" ref="C14:D14" si="9">C3+C4+C5+C6</f>
         <v>-96.835599999999985</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-5107.7600999999995</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-694.7553333333334</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
       <c r="H14" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>166.87423333333322</v>
       </c>
       <c r="I14" s="5"/>
@@ -1629,10 +1674,10 @@
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1645,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ19"/>
+  <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,31 +1845,31 @@
       <c r="D3" s="3">
         <v>8679.0730000000003</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="11">
         <v>-1618.1489999999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="11">
         <v>453.10359999999997</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="11">
         <v>490.26949999999999</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="11">
         <v>367.83620000000002</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="11">
         <v>265.60359999999997</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="11">
         <v>-70.117949999999993</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="11">
         <v>121.5496</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="11">
         <v>217.6498</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="11">
         <v>-51.80359</v>
       </c>
       <c r="O3" t="s">
@@ -1907,40 +1952,40 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="11">
         <v>180.05250000000001</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="11">
         <v>-498.89830000000001</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="11">
         <v>1226.9100000000001</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="11">
         <v>289.29090000000002</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="11">
         <v>195.8038</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="11">
         <v>547.39380000000006</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="11">
         <v>442.00060000000002</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="11">
         <v>-128.5812</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="11">
         <v>-133.49080000000001</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="11">
         <v>-20.370909999999999</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="11">
         <v>46.600340000000003</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="11">
         <v>-91.715239999999994</v>
       </c>
       <c r="O4" t="s">
@@ -1965,7 +2010,7 @@
         <v>9312.2900000000009</v>
       </c>
       <c r="V4" s="1">
-        <v>-20798.7</v>
+        <v>-867.976</v>
       </c>
       <c r="W4" s="2">
         <v>-20400.5</v>
@@ -2026,40 +2071,40 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="11">
         <v>-31.674469999999999</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="11">
         <v>214.5676</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <v>-250.47909999999999</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="11">
         <v>130.35220000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="11">
         <v>38.012700000000002</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="11">
         <v>-343.2747</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="11">
         <v>104.08920000000001</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="11">
         <v>12.853999999999999</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="11">
         <v>-480.74110000000002</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="11">
         <v>-461.38709999999998</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="11">
         <v>-78.231809999999996</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="11">
         <v>393.67899999999997</v>
       </c>
       <c r="O5" t="s">
@@ -2130,7 +2175,7 @@
       </c>
       <c r="AL5">
         <f t="shared" si="0"/>
-        <v>-19757.310000000001</v>
+        <v>173.4140000000001</v>
       </c>
       <c r="AM5">
         <f t="shared" si="0"/>
@@ -2157,40 +2202,40 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="11">
         <v>113.0776</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="11">
         <v>-72.866820000000004</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <v>28.23563</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="11">
         <v>-41.543100000000003</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="11">
         <v>-49.461359999999999</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="11">
         <v>126.5671</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="11">
         <v>-180.99440000000001</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="11">
         <v>14.089969999999999</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="11">
         <v>257.24259999999998</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="11">
         <v>251.55950000000001</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="11">
         <v>18.29224</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="11">
         <v>-188.6063</v>
       </c>
       <c r="O6" t="s">
@@ -2434,13 +2479,22 @@
         <f t="shared" si="4"/>
         <v>9088.0429999999997</v>
       </c>
-      <c r="E12" s="4">
-        <f>B4+E4/3</f>
-        <v>276.4828</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="E12" s="1">
+        <f>B11+(B4+E3+E4/3)/3</f>
+        <v>-532.45987666666667</v>
+      </c>
+      <c r="F12" s="1">
+        <f>C11+(C4+F3+F4/3)/3</f>
+        <v>-20647.518922222222</v>
+      </c>
+      <c r="G12" s="1">
+        <f>D11+(D4+G3+G4/3)/3</f>
+        <v>9312.2877000000008</v>
+      </c>
+      <c r="H12">
+        <f>(B4+E4+E3+H3+H4/3)/3</f>
+        <v>-211.21195555555553</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2499,22 +2553,37 @@
       <c r="L14" s="5"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <f>E4/3</f>
-        <v>96.430300000000003</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19">
-        <f>-(S3-S4)</f>
-        <v>92.160999999999945</v>
+        <f>-(V3-V4)</f>
+        <v>173.4140000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f>-(S4-V4)</f>
+        <v>-335.51599999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>-(P3-V4)</f>
+        <v>-782.73820000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2528,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2539,7 +2608,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>